<commit_message>
first block of moving DumpShort functions
</commit_message>
<xml_diff>
--- a/images/SIUnitPrefixTable.xlsx
+++ b/images/SIUnitPrefixTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenroe/Dropbox/DockerWorld/raku-Physics-Measure-v0.0.3/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E62F2042-DB66-8047-920C-8BDFB13170BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C073A8A-F330-CD46-B75F-009432BA84D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="60" windowWidth="28040" windowHeight="17440" xr2:uid="{543DC9AE-4713-E547-BEF5-C8E53014BAAD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>    'da', 'deka',</t>
   </si>
@@ -185,7 +185,22 @@
     <t>SI Derived Unit (20)</t>
   </si>
   <si>
-    <t>#added due to common use of ml, dl, etc. </t>
+    <t>:DEFAULT</t>
+  </si>
+  <si>
+    <t>:ALL</t>
+  </si>
+  <si>
+    <t>:electrical</t>
+  </si>
+  <si>
+    <t>:mechanical</t>
+  </si>
+  <si>
+    <t>:special</t>
+  </si>
+  <si>
+    <t>#litre added due to common use of ml, dl, etc. </t>
   </si>
 </sst>
 </file>
@@ -223,12 +238,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCFFA8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE4B5DB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -243,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -251,12 +290,26 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFE4B5DB"/>
+      <color rgb="FFFCFFA8"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -568,7 +621,7 @@
   <dimension ref="B2:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -590,10 +643,10 @@
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -601,10 +654,10 @@
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="11" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -612,10 +665,10 @@
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="11" t="s">
         <v>30</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -623,10 +676,10 @@
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="11" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -634,10 +687,10 @@
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="11" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -645,10 +698,10 @@
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -656,10 +709,10 @@
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="7" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -667,7 +720,7 @@
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -675,7 +728,7 @@
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -683,7 +736,7 @@
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="7" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -691,7 +744,7 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="7" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -699,7 +752,10 @@
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C14" s="1" t="s">
+      <c r="B14" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -707,7 +763,10 @@
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C15" s="1" t="s">
+      <c r="B15" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -715,64 +774,73 @@
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C16" s="1" t="s">
+      <c r="B16" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>41</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C17" s="1" t="s">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>42</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C18" s="1" t="s">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C19" s="1" t="s">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C19" s="10" t="s">
         <v>44</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C20" s="1" t="s">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C20" s="10" t="s">
         <v>45</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C21" s="1" t="s">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C21" s="10" t="s">
         <v>46</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C22" s="1" t="s">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C22" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C23" s="4" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed pi to π
</commit_message>
<xml_diff>
--- a/images/SIUnitPrefixTable.xlsx
+++ b/images/SIUnitPrefixTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenroe/Dropbox/DockerWorld/raku-Physics-Measure-v0.0.3/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C073A8A-F330-CD46-B75F-009432BA84D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD1D0AE-0B5C-6148-9143-0182E21F421B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="60" windowWidth="28040" windowHeight="17440" xr2:uid="{543DC9AE-4713-E547-BEF5-C8E53014BAAD}"/>
+    <workbookView xWindow="30280" yWindow="1180" windowWidth="28040" windowHeight="17440" xr2:uid="{543DC9AE-4713-E547-BEF5-C8E53014BAAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -197,10 +197,10 @@
     <t>:mechanical</t>
   </si>
   <si>
-    <t>:special</t>
-  </si>
-  <si>
     <t>#litre added due to common use of ml, dl, etc. </t>
+  </si>
+  <si>
+    <t>:astral</t>
   </si>
 </sst>
 </file>
@@ -621,7 +621,7 @@
   <dimension ref="B2:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -786,7 +786,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>42</v>
@@ -840,7 +840,7 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C23" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>